<commit_message>
Fixed Omission of Main PCB in BOME PDF
The print area was not correct in the XLS which then omitted the Main PCB.  It has been updated.
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -9,13 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="14655"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="14652"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$9:$G$126</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$G$126</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -801,23 +801,23 @@
   </sheetPr>
   <dimension ref="A1:G126"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:G126"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.88671875" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="89" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="165.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="1"/>
+    <col min="7" max="7" width="165.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>30</v>
       </c>
@@ -828,7 +828,7 @@
       <c r="F1" s="7"/>
       <c r="G1" s="7"/>
     </row>
-    <row r="2" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
@@ -851,7 +851,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>37</v>
       </c>
@@ -872,7 +872,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:7" s="10" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" s="10" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
         <v>31</v>
       </c>
@@ -893,7 +893,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="5" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>62</v>
       </c>
@@ -914,7 +914,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>65</v>
       </c>
@@ -935,7 +935,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>33</v>
       </c>
@@ -956,7 +956,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
@@ -965,7 +965,7 @@
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
     </row>
-    <row r="9" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
         <v>13</v>
       </c>
@@ -976,7 +976,7 @@
       <c r="F9" s="7"/>
       <c r="G9" s="7"/>
     </row>
-    <row r="10" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>0</v>
       </c>
@@ -999,7 +999,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>40</v>
       </c>
@@ -1020,7 +1020,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="12" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>9</v>
       </c>
@@ -1041,7 +1041,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="13" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2" t="s">
@@ -1058,7 +1058,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
@@ -1067,7 +1067,7 @@
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
     </row>
-    <row r="15" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="s">
         <v>97</v>
       </c>
@@ -1078,7 +1078,7 @@
       <c r="F15" s="7"/>
       <c r="G15" s="7"/>
     </row>
-    <row r="16" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
         <v>0</v>
       </c>
@@ -1101,7 +1101,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>40</v>
       </c>
@@ -1122,7 +1122,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="18" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>9</v>
       </c>
@@ -1143,7 +1143,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="19" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2" t="s">
@@ -1160,7 +1160,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="20" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
@@ -1169,7 +1169,7 @@
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
     </row>
-    <row r="21" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21" s="7" t="s">
         <v>96</v>
       </c>
@@ -1180,7 +1180,7 @@
       <c r="F21" s="7"/>
       <c r="G21" s="7"/>
     </row>
-    <row r="22" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
         <v>0</v>
       </c>
@@ -1203,7 +1203,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>40</v>
       </c>
@@ -1224,7 +1224,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="24" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>9</v>
       </c>
@@ -1245,7 +1245,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="25" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2" t="s">
@@ -1262,7 +1262,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="26" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A26" s="3"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
@@ -1271,7 +1271,7 @@
       <c r="F26" s="3"/>
       <c r="G26" s="3"/>
     </row>
-    <row r="27" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A27" s="7" t="s">
         <v>94</v>
       </c>
@@ -1282,7 +1282,7 @@
       <c r="F27" s="7"/>
       <c r="G27" s="7"/>
     </row>
-    <row r="28" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A28" s="4" t="s">
         <v>0</v>
       </c>
@@ -1305,7 +1305,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>40</v>
       </c>
@@ -1326,7 +1326,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="30" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>9</v>
       </c>
@@ -1347,7 +1347,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="31" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A31" s="2"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2" t="s">
@@ -1362,7 +1362,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="32" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A32" s="3"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
@@ -1371,7 +1371,7 @@
       <c r="F32" s="3"/>
       <c r="G32" s="3"/>
     </row>
-    <row r="33" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A33" s="7" t="s">
         <v>95</v>
       </c>
@@ -1382,7 +1382,7 @@
       <c r="F33" s="7"/>
       <c r="G33" s="7"/>
     </row>
-    <row r="34" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A34" s="4" t="s">
         <v>0</v>
       </c>
@@ -1405,7 +1405,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="35" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>40</v>
       </c>
@@ -1426,7 +1426,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="36" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A36" s="2"/>
       <c r="B36" s="2"/>
       <c r="C36" s="2" t="s">
@@ -1443,7 +1443,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="37" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A37" s="3"/>
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
@@ -1452,7 +1452,7 @@
       <c r="F37" s="3"/>
       <c r="G37" s="3"/>
     </row>
-    <row r="38" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A38" s="7" t="s">
         <v>29</v>
       </c>
@@ -1463,7 +1463,7 @@
       <c r="F38" s="7"/>
       <c r="G38" s="7"/>
     </row>
-    <row r="39" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A39" s="4" t="s">
         <v>0</v>
       </c>
@@ -1486,7 +1486,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="40" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
         <v>40</v>
       </c>
@@ -1507,7 +1507,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="41" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A41" s="2"/>
       <c r="B41" s="2"/>
       <c r="C41" s="2" t="s">
@@ -1524,7 +1524,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="42" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A42" s="3"/>
       <c r="B42" s="3"/>
       <c r="C42" s="3"/>
@@ -1533,7 +1533,7 @@
       <c r="F42" s="3"/>
       <c r="G42" s="3"/>
     </row>
-    <row r="43" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A43" s="7" t="s">
         <v>98</v>
       </c>
@@ -1544,7 +1544,7 @@
       <c r="F43" s="7"/>
       <c r="G43" s="7"/>
     </row>
-    <row r="44" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A44" s="4" t="s">
         <v>0</v>
       </c>
@@ -1567,7 +1567,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="45" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
         <v>40</v>
       </c>
@@ -1588,7 +1588,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="46" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
         <v>9</v>
       </c>
@@ -1609,7 +1609,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="47" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A47" s="2"/>
       <c r="B47" s="2"/>
       <c r="C47" s="2" t="s">
@@ -1626,7 +1626,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="48" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A48" s="3"/>
       <c r="B48" s="3"/>
       <c r="C48" s="3"/>
@@ -1635,7 +1635,7 @@
       <c r="F48" s="3"/>
       <c r="G48" s="3"/>
     </row>
-    <row r="49" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A49" s="7" t="s">
         <v>99</v>
       </c>
@@ -1646,7 +1646,7 @@
       <c r="F49" s="7"/>
       <c r="G49" s="7"/>
     </row>
-    <row r="50" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A50" s="4" t="s">
         <v>0</v>
       </c>
@@ -1669,7 +1669,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="51" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
         <v>40</v>
       </c>
@@ -1690,7 +1690,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="52" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
         <v>9</v>
       </c>
@@ -1711,7 +1711,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="53" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
         <v>109</v>
       </c>
@@ -1732,7 +1732,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="54" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
         <v>110</v>
       </c>
@@ -1753,7 +1753,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="55" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A55" s="2"/>
       <c r="B55" s="2"/>
       <c r="C55" s="2" t="s">
@@ -1770,7 +1770,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="56" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A56" s="3"/>
       <c r="B56" s="3"/>
       <c r="C56" s="3"/>
@@ -1779,7 +1779,7 @@
       <c r="F56" s="3"/>
       <c r="G56" s="3"/>
     </row>
-    <row r="57" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A57" s="7" t="s">
         <v>100</v>
       </c>
@@ -1790,7 +1790,7 @@
       <c r="F57" s="7"/>
       <c r="G57" s="7"/>
     </row>
-    <row r="58" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A58" s="4" t="s">
         <v>0</v>
       </c>
@@ -1813,7 +1813,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="59" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="s">
         <v>40</v>
       </c>
@@ -1834,7 +1834,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="60" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A60" s="2" t="s">
         <v>9</v>
       </c>
@@ -1855,7 +1855,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="61" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A61" s="2"/>
       <c r="B61" s="2"/>
       <c r="C61" s="2" t="s">
@@ -1870,7 +1870,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="62" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A62" s="3"/>
       <c r="B62" s="3"/>
       <c r="C62" s="3"/>
@@ -1879,7 +1879,7 @@
       <c r="F62" s="3"/>
       <c r="G62" s="3"/>
     </row>
-    <row r="63" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A63" s="7" t="s">
         <v>101</v>
       </c>
@@ -1890,7 +1890,7 @@
       <c r="F63" s="7"/>
       <c r="G63" s="7"/>
     </row>
-    <row r="64" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A64" s="4" t="s">
         <v>0</v>
       </c>
@@ -1913,7 +1913,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="65" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A65" s="2" t="s">
         <v>40</v>
       </c>
@@ -1934,7 +1934,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="66" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A66" s="2" t="s">
         <v>9</v>
       </c>
@@ -1955,7 +1955,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="67" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A67" s="2"/>
       <c r="B67" s="2"/>
       <c r="C67" s="2" t="s">
@@ -1970,7 +1970,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="68" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A68" s="3"/>
       <c r="B68" s="3"/>
       <c r="C68" s="3"/>
@@ -1979,7 +1979,7 @@
       <c r="F68" s="3"/>
       <c r="G68" s="3"/>
     </row>
-    <row r="69" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A69" s="7" t="s">
         <v>11</v>
       </c>
@@ -1990,7 +1990,7 @@
       <c r="F69" s="7"/>
       <c r="G69" s="7"/>
     </row>
-    <row r="70" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A70" s="4" t="s">
         <v>0</v>
       </c>
@@ -2013,7 +2013,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="71" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A71" s="2" t="s">
         <v>40</v>
       </c>
@@ -2034,7 +2034,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="72" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A72" s="2" t="s">
         <v>9</v>
       </c>
@@ -2055,7 +2055,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="73" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A73" s="2" t="s">
         <v>50</v>
       </c>
@@ -2078,7 +2078,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="74" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A74" s="2"/>
       <c r="B74" s="2"/>
       <c r="C74" s="2" t="s">
@@ -2095,7 +2095,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="75" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A75" s="3"/>
       <c r="B75" s="3"/>
       <c r="C75" s="3"/>
@@ -2104,7 +2104,7 @@
       <c r="F75" s="3"/>
       <c r="G75" s="3"/>
     </row>
-    <row r="76" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A76" s="7" t="s">
         <v>28</v>
       </c>
@@ -2115,7 +2115,7 @@
       <c r="F76" s="7"/>
       <c r="G76" s="7"/>
     </row>
-    <row r="77" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A77" s="4" t="s">
         <v>0</v>
       </c>
@@ -2138,7 +2138,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="78" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A78" s="2" t="s">
         <v>40</v>
       </c>
@@ -2159,7 +2159,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="79" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A79" s="2"/>
       <c r="B79" s="2"/>
       <c r="C79" s="2" t="s">
@@ -2176,7 +2176,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="80" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A80" s="3"/>
       <c r="B80" s="3"/>
       <c r="C80" s="3"/>
@@ -2185,7 +2185,7 @@
       <c r="F80" s="3"/>
       <c r="G80" s="3"/>
     </row>
-    <row r="81" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A81" s="7" t="s">
         <v>14</v>
       </c>
@@ -2196,7 +2196,7 @@
       <c r="F81" s="7"/>
       <c r="G81" s="7"/>
     </row>
-    <row r="82" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A82" s="4" t="s">
         <v>0</v>
       </c>
@@ -2219,7 +2219,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="83" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A83" s="2" t="s">
         <v>40</v>
       </c>
@@ -2240,7 +2240,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="84" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A84" s="2" t="s">
         <v>9</v>
       </c>
@@ -2261,7 +2261,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="85" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A85" s="2" t="s">
         <v>44</v>
       </c>
@@ -2282,7 +2282,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="86" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A86" s="2"/>
       <c r="B86" s="2"/>
       <c r="C86" s="2" t="s">
@@ -2299,7 +2299,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="87" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A87" s="2"/>
       <c r="B87" s="2"/>
       <c r="C87" s="2"/>
@@ -2312,7 +2312,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="88" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A88" s="3"/>
       <c r="B88" s="3"/>
       <c r="C88" s="3"/>
@@ -2321,7 +2321,7 @@
       <c r="F88" s="3"/>
       <c r="G88" s="3"/>
     </row>
-    <row r="89" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A89" s="7" t="s">
         <v>102</v>
       </c>
@@ -2332,7 +2332,7 @@
       <c r="F89" s="7"/>
       <c r="G89" s="7"/>
     </row>
-    <row r="90" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A90" s="4" t="s">
         <v>0</v>
       </c>
@@ -2355,7 +2355,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="91" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A91" s="2" t="s">
         <v>40</v>
       </c>
@@ -2376,7 +2376,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="92" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A92" s="2" t="s">
         <v>9</v>
       </c>
@@ -2397,7 +2397,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="93" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A93" s="2"/>
       <c r="B93" s="2"/>
       <c r="C93" s="2" t="s">
@@ -2414,7 +2414,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="94" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A94" s="3"/>
       <c r="B94" s="3"/>
       <c r="C94" s="3"/>
@@ -2423,7 +2423,7 @@
       <c r="F94" s="3"/>
       <c r="G94" s="3"/>
     </row>
-    <row r="95" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A95" s="7" t="s">
         <v>15</v>
       </c>
@@ -2434,7 +2434,7 @@
       <c r="F95" s="7"/>
       <c r="G95" s="7"/>
     </row>
-    <row r="96" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A96" s="4" t="s">
         <v>0</v>
       </c>
@@ -2457,7 +2457,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="97" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A97" s="2" t="s">
         <v>40</v>
       </c>
@@ -2478,7 +2478,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="98" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A98" s="2"/>
       <c r="B98" s="2"/>
       <c r="C98" s="2" t="s">
@@ -2495,7 +2495,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="99" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A99" s="3"/>
       <c r="B99" s="3"/>
       <c r="C99" s="3"/>
@@ -2504,7 +2504,7 @@
       <c r="F99" s="3"/>
       <c r="G99" s="3"/>
     </row>
-    <row r="100" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A100" s="7" t="s">
         <v>16</v>
       </c>
@@ -2515,7 +2515,7 @@
       <c r="F100" s="7"/>
       <c r="G100" s="7"/>
     </row>
-    <row r="101" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A101" s="4" t="s">
         <v>0</v>
       </c>
@@ -2538,7 +2538,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="102" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A102" s="2" t="s">
         <v>40</v>
       </c>
@@ -2559,7 +2559,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="103" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A103" s="2" t="s">
         <v>9</v>
       </c>
@@ -2580,7 +2580,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="104" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A104" s="2"/>
       <c r="B104" s="2"/>
       <c r="C104" s="2" t="s">
@@ -2595,7 +2595,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="105" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A105" s="3"/>
       <c r="B105" s="3"/>
       <c r="C105" s="3"/>
@@ -2604,7 +2604,7 @@
       <c r="F105" s="3"/>
       <c r="G105" s="3"/>
     </row>
-    <row r="106" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A106" s="7" t="s">
         <v>103</v>
       </c>
@@ -2615,7 +2615,7 @@
       <c r="F106" s="7"/>
       <c r="G106" s="7"/>
     </row>
-    <row r="107" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A107" s="4" t="s">
         <v>0</v>
       </c>
@@ -2638,7 +2638,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="108" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A108" s="2" t="s">
         <v>40</v>
       </c>
@@ -2659,7 +2659,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="109" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A109" s="2" t="s">
         <v>9</v>
       </c>
@@ -2680,7 +2680,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="110" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A110" s="2"/>
       <c r="B110" s="2"/>
       <c r="C110" s="2" t="s">
@@ -2697,7 +2697,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="111" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A111" s="3"/>
       <c r="B111" s="3"/>
       <c r="C111" s="3"/>
@@ -2706,7 +2706,7 @@
       <c r="F111" s="3"/>
       <c r="G111" s="3"/>
     </row>
-    <row r="112" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A112" s="7" t="s">
         <v>104</v>
       </c>
@@ -2717,7 +2717,7 @@
       <c r="F112" s="7"/>
       <c r="G112" s="7"/>
     </row>
-    <row r="113" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A113" s="4" t="s">
         <v>0</v>
       </c>
@@ -2740,7 +2740,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="114" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A114" s="2" t="s">
         <v>40</v>
       </c>
@@ -2761,7 +2761,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="115" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A115" s="2" t="s">
         <v>9</v>
       </c>
@@ -2782,7 +2782,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="116" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A116" s="2"/>
       <c r="B116" s="2"/>
       <c r="C116" s="2" t="s">
@@ -2797,7 +2797,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="117" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A117" s="3"/>
       <c r="B117" s="3"/>
       <c r="C117" s="3"/>
@@ -2806,7 +2806,7 @@
       <c r="F117" s="3"/>
       <c r="G117" s="3"/>
     </row>
-    <row r="118" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A118" s="7" t="s">
         <v>17</v>
       </c>
@@ -2817,7 +2817,7 @@
       <c r="F118" s="7"/>
       <c r="G118" s="7"/>
     </row>
-    <row r="119" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A119" s="4" t="s">
         <v>0</v>
       </c>
@@ -2840,7 +2840,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="120" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A120" s="2" t="s">
         <v>40</v>
       </c>
@@ -2861,7 +2861,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="121" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A121" s="2" t="s">
         <v>9</v>
       </c>
@@ -2882,7 +2882,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="122" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A122" s="2" t="s">
         <v>69</v>
       </c>
@@ -2903,7 +2903,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="123" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A123" s="2" t="s">
         <v>20</v>
       </c>
@@ -2924,7 +2924,7 @@
       </c>
       <c r="G123" s="2"/>
     </row>
-    <row r="124" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A124" s="2" t="s">
         <v>23</v>
       </c>
@@ -2945,7 +2945,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="125" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A125" s="2" t="s">
         <v>27</v>
       </c>
@@ -2964,7 +2964,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="126" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A126" s="2"/>
       <c r="B126" s="2"/>
       <c r="C126" s="2" t="s">
@@ -3044,6 +3044,6 @@
     <hyperlink ref="G31" r:id="rId59"/>
   </hyperlinks>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="41" fitToHeight="0" orientation="landscape" r:id="rId60"/>
+  <pageSetup scale="38" fitToHeight="0" orientation="landscape" r:id="rId60"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Wii Ext, NES/SNES Mini PCB Design Status
Design is complete, updating BOM and project Status before merging.
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -15,7 +15,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$G$127</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$G$133</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -845,7 +845,7 @@
   <dimension ref="A1:G133"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F133" sqref="F133"/>
+      <selection sqref="A1:G133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Updated BOM for SNES Multitap Clarity
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\Blue-Retro-AIO-Units\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24332ECE-C32A-4F09-9E99-EFFD734F1B7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="14655" activeTab="1"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PCB Parts and Cables" sheetId="1" r:id="rId1"/>
@@ -17,7 +18,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="1">'3D Printed Parts'!$A$1:$A$66</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'PCB Parts and Cables'!$A$1:$G$135</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'PCB Parts and Cables'!$A$1:$G$136</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="550" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="552" uniqueCount="181">
   <si>
     <t>Part #</t>
   </si>
@@ -376,9 +377,6 @@
     <t>RMCF1206JT1K00</t>
   </si>
   <si>
-    <t>https://www.amazon.com/TENINYU-Controller-Extension-Versions-Nintendo/dp/B07H1J71XR/ref=sr_1_8?keywords=wii+extension+cable&amp;qid=1668461824&amp;sprefix=wii+exten%2Caps%2C119&amp;sr=8-8</t>
-  </si>
-  <si>
     <t>SNES/NES Mini Extension</t>
   </si>
   <si>
@@ -563,12 +561,24 @@
   </si>
   <si>
     <t>Aux Top - Nintendo Wii or Aux Top - Nintendo Wii Ext or Aux Top - Nintendo SNES Classic or Aux Top - Nintendo SFC Classic or Aux Top - Nintendo NES Classic or Aux Top - Nintendo Famicom Classic</t>
+  </si>
+  <si>
+    <t>https://console5.com/store/snes-controller-extension-cable-6-foot-1-8m.html</t>
+  </si>
+  <si>
+    <t>Can Find Different options on Amazon, This is not a 7 Conductor Cable. For Multitap follow Darthcloud's Instructions:</t>
+  </si>
+  <si>
+    <t>SNES controller plug (x2) (For multitap support 7 conductor are required, get a 3rd SNES extension for pin donation and use cable from PSX/Genesis/Saturn for the extra wires)</t>
+  </si>
+  <si>
+    <t>https://a.co/d/1FtFBEe</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -606,7 +616,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -640,27 +650,47 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -668,6 +698,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -948,14 +987,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G135"/>
+  <dimension ref="A1:G136"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A82" sqref="A82"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A7" zoomScale="60" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G85" sqref="G85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -966,20 +1005,20 @@
     <col min="4" max="4" width="5.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="89" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="165.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="152.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
     </row>
     <row r="2" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
@@ -1004,7 +1043,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>27</v>
       </c>
@@ -1025,30 +1064,30 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:7" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
+    <row r="4" spans="1:7" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="B4" s="7" t="s">
         <v>118</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="C4" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="C4" s="8" t="s">
-        <v>120</v>
-      </c>
-      <c r="D4" s="8">
-        <v>1</v>
-      </c>
-      <c r="E4" s="8" t="s">
+      <c r="D4" s="7">
+        <v>1</v>
+      </c>
+      <c r="E4" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="F4" s="8" t="s">
+      <c r="F4" s="7" t="s">
         <v>21</v>
       </c>
       <c r="G4" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="5" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>52</v>
       </c>
@@ -1069,7 +1108,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>55</v>
       </c>
@@ -1090,7 +1129,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>23</v>
       </c>
@@ -1111,7 +1150,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
@@ -1121,15 +1160,15 @@
       <c r="G8" s="3"/>
     </row>
     <row r="9" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="7" t="s">
+      <c r="A9" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
     </row>
     <row r="10" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
@@ -1154,7 +1193,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>30</v>
       </c>
@@ -1175,7 +1214,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>9</v>
       </c>
@@ -1196,7 +1235,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2" t="s">
@@ -1213,7 +1252,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
@@ -1223,15 +1262,15 @@
       <c r="G14" s="3"/>
     </row>
     <row r="15" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="7" t="s">
+      <c r="A15" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="B15" s="7"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="7"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
     </row>
     <row r="16" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
@@ -1256,7 +1295,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>30</v>
       </c>
@@ -1277,7 +1316,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>9</v>
       </c>
@@ -1298,7 +1337,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2" t="s">
@@ -1315,7 +1354,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="20" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
@@ -1325,15 +1364,15 @@
       <c r="G20" s="3"/>
     </row>
     <row r="21" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="B21" s="7"/>
-      <c r="C21" s="7"/>
-      <c r="D21" s="7"/>
-      <c r="E21" s="7"/>
-      <c r="F21" s="7"/>
-      <c r="G21" s="7"/>
+      <c r="A21" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="B21" s="6"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6"/>
     </row>
     <row r="22" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
@@ -1358,7 +1397,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>30</v>
       </c>
@@ -1379,7 +1418,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="24" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>9</v>
       </c>
@@ -1400,7 +1439,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="25" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2" t="s">
@@ -1411,11 +1450,11 @@
       </c>
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
-      <c r="G25" s="10" t="s">
+      <c r="G25" s="2" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="26" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="3"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
@@ -1425,15 +1464,15 @@
       <c r="G26" s="3"/>
     </row>
     <row r="27" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="7" t="s">
-        <v>162</v>
-      </c>
-      <c r="B27" s="7"/>
-      <c r="C27" s="7"/>
-      <c r="D27" s="7"/>
-      <c r="E27" s="7"/>
-      <c r="F27" s="7"/>
-      <c r="G27" s="7"/>
+      <c r="A27" s="6" t="s">
+        <v>161</v>
+      </c>
+      <c r="B27" s="6"/>
+      <c r="C27" s="6"/>
+      <c r="D27" s="6"/>
+      <c r="E27" s="6"/>
+      <c r="F27" s="6"/>
+      <c r="G27" s="6"/>
     </row>
     <row r="28" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
@@ -1458,7 +1497,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>30</v>
       </c>
@@ -1479,7 +1518,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="30" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>9</v>
       </c>
@@ -1500,7 +1539,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="31" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>34</v>
       </c>
@@ -1521,7 +1560,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="32" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="2"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2" t="s">
@@ -1538,7 +1577,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="33" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="2"/>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
@@ -1551,7 +1590,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="34" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="3"/>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
@@ -1561,15 +1600,15 @@
       <c r="G34" s="3"/>
     </row>
     <row r="35" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="7" t="s">
-        <v>161</v>
-      </c>
-      <c r="B35" s="7"/>
-      <c r="C35" s="7"/>
-      <c r="D35" s="7"/>
-      <c r="E35" s="7"/>
-      <c r="F35" s="7"/>
-      <c r="G35" s="7"/>
+      <c r="A35" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="B35" s="6"/>
+      <c r="C35" s="6"/>
+      <c r="D35" s="6"/>
+      <c r="E35" s="6"/>
+      <c r="F35" s="6"/>
+      <c r="G35" s="6"/>
     </row>
     <row r="36" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
@@ -1594,7 +1633,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="37" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>30</v>
       </c>
@@ -1615,7 +1654,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="38" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>9</v>
       </c>
@@ -1636,7 +1675,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="39" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="2"/>
       <c r="B39" s="2"/>
       <c r="C39" s="2" t="s">
@@ -1653,7 +1692,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="40" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="3"/>
       <c r="B40" s="3"/>
       <c r="C40" s="3"/>
@@ -1663,15 +1702,15 @@
       <c r="G40" s="3"/>
     </row>
     <row r="41" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="7" t="s">
+      <c r="A41" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B41" s="7"/>
-      <c r="C41" s="7"/>
-      <c r="D41" s="7"/>
-      <c r="E41" s="7"/>
-      <c r="F41" s="7"/>
-      <c r="G41" s="7"/>
+      <c r="B41" s="6"/>
+      <c r="C41" s="6"/>
+      <c r="D41" s="6"/>
+      <c r="E41" s="6"/>
+      <c r="F41" s="6"/>
+      <c r="G41" s="6"/>
     </row>
     <row r="42" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
@@ -1696,7 +1735,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="43" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>30</v>
       </c>
@@ -1717,7 +1756,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="44" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="2"/>
       <c r="B44" s="2"/>
       <c r="C44" s="2" t="s">
@@ -1734,7 +1773,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="45" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="3"/>
       <c r="B45" s="3"/>
       <c r="C45" s="3"/>
@@ -1744,15 +1783,15 @@
       <c r="G45" s="3"/>
     </row>
     <row r="46" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="7" t="s">
-        <v>146</v>
-      </c>
-      <c r="B46" s="7"/>
-      <c r="C46" s="7"/>
-      <c r="D46" s="7"/>
-      <c r="E46" s="7"/>
-      <c r="F46" s="7"/>
-      <c r="G46" s="7"/>
+      <c r="A46" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="B46" s="6"/>
+      <c r="C46" s="6"/>
+      <c r="D46" s="6"/>
+      <c r="E46" s="6"/>
+      <c r="F46" s="6"/>
+      <c r="G46" s="6"/>
     </row>
     <row r="47" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
@@ -1777,7 +1816,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="48" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>30</v>
       </c>
@@ -1798,7 +1837,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="49" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="2"/>
       <c r="B49" s="2"/>
       <c r="C49" s="2" t="s">
@@ -1815,7 +1854,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="50" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="3"/>
       <c r="B50" s="3"/>
       <c r="C50" s="3"/>
@@ -1825,15 +1864,15 @@
       <c r="G50" s="3"/>
     </row>
     <row r="51" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="7" t="s">
-        <v>147</v>
-      </c>
-      <c r="B51" s="7"/>
-      <c r="C51" s="7"/>
-      <c r="D51" s="7"/>
-      <c r="E51" s="7"/>
-      <c r="F51" s="7"/>
-      <c r="G51" s="7"/>
+      <c r="A51" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="B51" s="6"/>
+      <c r="C51" s="6"/>
+      <c r="D51" s="6"/>
+      <c r="E51" s="6"/>
+      <c r="F51" s="6"/>
+      <c r="G51" s="6"/>
     </row>
     <row r="52" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
@@ -1858,7 +1897,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="53" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
         <v>30</v>
       </c>
@@ -1879,7 +1918,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="54" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
         <v>9</v>
       </c>
@@ -1900,7 +1939,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="55" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
         <v>40</v>
       </c>
@@ -1923,7 +1962,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="56" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="2"/>
       <c r="B56" s="2"/>
       <c r="C56" s="2" t="s">
@@ -1940,7 +1979,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="57" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="3"/>
       <c r="B57" s="3"/>
       <c r="C57" s="3"/>
@@ -1950,15 +1989,15 @@
       <c r="G57" s="3"/>
     </row>
     <row r="58" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="7" t="s">
-        <v>148</v>
-      </c>
-      <c r="B58" s="7"/>
-      <c r="C58" s="7"/>
-      <c r="D58" s="7"/>
-      <c r="E58" s="7"/>
-      <c r="F58" s="7"/>
-      <c r="G58" s="7"/>
+      <c r="A58" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="B58" s="6"/>
+      <c r="C58" s="6"/>
+      <c r="D58" s="6"/>
+      <c r="E58" s="6"/>
+      <c r="F58" s="6"/>
+      <c r="G58" s="6"/>
     </row>
     <row r="59" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
@@ -1983,7 +2022,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="60" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
         <v>30</v>
       </c>
@@ -2004,7 +2043,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="61" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
         <v>9</v>
       </c>
@@ -2025,203 +2064,199 @@
         <v>33</v>
       </c>
     </row>
-    <row r="62" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A62" s="2"/>
       <c r="B62" s="2"/>
       <c r="C62" s="2" t="s">
         <v>80</v>
       </c>
       <c r="D62" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E62" s="2"/>
-      <c r="F62" s="2"/>
-      <c r="G62" s="10" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="3"/>
-      <c r="B63" s="3"/>
-      <c r="C63" s="3"/>
-      <c r="D63" s="3"/>
-      <c r="E63" s="3"/>
-      <c r="F63" s="3"/>
-      <c r="G63" s="3"/>
-    </row>
-    <row r="64" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="7" t="s">
-        <v>149</v>
-      </c>
-      <c r="B64" s="7"/>
-      <c r="C64" s="7"/>
-      <c r="D64" s="7"/>
-      <c r="E64" s="7"/>
-      <c r="F64" s="7"/>
-      <c r="G64" s="7"/>
+      <c r="F62" s="9" t="s">
+        <v>178</v>
+      </c>
+      <c r="G62" s="13" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A63" s="2"/>
+      <c r="B63" s="2"/>
+      <c r="C63" s="2"/>
+      <c r="D63" s="2"/>
+      <c r="E63" s="2"/>
+      <c r="F63" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="G63" s="14"/>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A64" s="3"/>
+      <c r="B64" s="3"/>
+      <c r="C64" s="3"/>
+      <c r="D64" s="3"/>
+      <c r="E64" s="3"/>
+      <c r="F64" s="12"/>
+      <c r="G64" s="3"/>
     </row>
     <row r="65" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="4" t="s">
+      <c r="A65" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="B65" s="6"/>
+      <c r="C65" s="6"/>
+      <c r="D65" s="6"/>
+      <c r="E65" s="6"/>
+      <c r="F65" s="6"/>
+      <c r="G65" s="6"/>
+    </row>
+    <row r="66" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B65" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C65" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D65" s="4" t="s">
+      <c r="B66" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C66" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D66" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E65" s="4" t="s">
+      <c r="E66" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F65" s="4" t="s">
+      <c r="F66" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="G65" s="4" t="s">
+      <c r="G66" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="66" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="2" t="s">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A67" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B66" s="2" t="s">
+      <c r="B67" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C66" s="2" t="s">
+      <c r="C67" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D66" s="2">
-        <v>1</v>
-      </c>
-      <c r="E66" s="2" t="s">
+      <c r="D67" s="2">
+        <v>1</v>
+      </c>
+      <c r="E67" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="F66" s="2"/>
-      <c r="G66" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="67" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B67" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C67" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D67" s="2">
-        <v>2</v>
-      </c>
-      <c r="E67" s="2" t="s">
-        <v>38</v>
       </c>
       <c r="F67" s="2"/>
       <c r="G67" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="68" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
-        <v>59</v>
+        <v>9</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>60</v>
+        <v>8</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="D68" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>63</v>
+        <v>38</v>
       </c>
       <c r="F68" s="2"/>
       <c r="G68" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A69" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C69" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D69" s="2">
+        <v>1</v>
+      </c>
+      <c r="E69" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F69" s="2"/>
+      <c r="G69" s="2" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="69" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="2" t="s">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A70" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B69" s="2" t="s">
+      <c r="B70" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C69" s="2" t="s">
+      <c r="C70" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D69" s="2">
-        <v>1</v>
-      </c>
-      <c r="E69" s="2" t="s">
+      <c r="D70" s="2">
+        <v>1</v>
+      </c>
+      <c r="E70" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="F69" s="2" t="s">
+      <c r="F70" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="G69" s="2"/>
-    </row>
-    <row r="70" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="2" t="s">
+      <c r="G70" s="2"/>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A71" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B70" s="2" t="s">
+      <c r="B71" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C70" s="2" t="s">
+      <c r="C71" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D70" s="2">
-        <v>1</v>
-      </c>
-      <c r="E70" s="2" t="s">
+      <c r="D71" s="2">
+        <v>1</v>
+      </c>
+      <c r="E71" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="F70" s="2"/>
-      <c r="G70" s="2" t="s">
+      <c r="F71" s="2"/>
+      <c r="G71" s="2" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="71" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="2"/>
-      <c r="B71" s="2"/>
-      <c r="C71" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D71" s="2">
-        <v>1</v>
-      </c>
-      <c r="E71" s="2"/>
-      <c r="F71" s="2"/>
-      <c r="G71" s="10" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="72" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="11" t="s">
-        <v>126</v>
-      </c>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A72" s="2"/>
       <c r="B72" s="2"/>
       <c r="C72" s="2" t="s">
-        <v>124</v>
+        <v>18</v>
       </c>
       <c r="D72" s="2">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E72" s="2"/>
       <c r="F72" s="2"/>
-      <c r="G72" s="10" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="73" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="2" t="s">
+      <c r="G72" s="2" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A73" s="9" t="s">
         <v>125</v>
       </c>
       <c r="B73" s="2"/>
@@ -2229,1484 +2264,1508 @@
         <v>123</v>
       </c>
       <c r="D73" s="2">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E73" s="2"/>
       <c r="F73" s="2"/>
-      <c r="G73" s="10" t="s">
+      <c r="G73" s="2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A74" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="B74" s="2"/>
+      <c r="C74" s="2" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="74" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="7" t="s">
-        <v>150</v>
-      </c>
-      <c r="B74" s="7"/>
-      <c r="C74" s="7"/>
-      <c r="D74" s="7"/>
-      <c r="E74" s="7"/>
-      <c r="F74" s="7"/>
-      <c r="G74" s="7"/>
-    </row>
-    <row r="75" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="4" t="s">
+      <c r="D74" s="2">
+        <v>1</v>
+      </c>
+      <c r="E74" s="2"/>
+      <c r="F74" s="2"/>
+      <c r="G74" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A75" s="3"/>
+      <c r="B75" s="3"/>
+      <c r="C75" s="3"/>
+      <c r="D75" s="3"/>
+      <c r="E75" s="3"/>
+      <c r="F75" s="12"/>
+      <c r="G75" s="3"/>
+    </row>
+    <row r="76" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="B76" s="6"/>
+      <c r="C76" s="6"/>
+      <c r="D76" s="6"/>
+      <c r="E76" s="6"/>
+      <c r="F76" s="6"/>
+      <c r="G76" s="6"/>
+    </row>
+    <row r="77" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A77" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B75" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C75" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D75" s="4" t="s">
+      <c r="B77" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C77" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D77" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E75" s="4" t="s">
+      <c r="E77" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F75" s="4" t="s">
+      <c r="F77" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="G75" s="4" t="s">
+      <c r="G77" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="76" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="2" t="s">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A78" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B76" s="2" t="s">
+      <c r="B78" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C76" s="2" t="s">
+      <c r="C78" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D76" s="2">
-        <v>1</v>
-      </c>
-      <c r="E76" s="2" t="s">
+      <c r="D78" s="2">
+        <v>1</v>
+      </c>
+      <c r="E78" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="F76" s="2"/>
-      <c r="G76" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="77" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="B77" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="C77" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="D77" s="2">
-        <v>4</v>
-      </c>
-      <c r="E77" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="F77" s="2"/>
-      <c r="G77" s="2" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="78" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="11" t="s">
-        <v>111</v>
-      </c>
-      <c r="B78" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="C78" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="D78" s="2">
-        <v>1</v>
-      </c>
-      <c r="E78" s="2" t="s">
-        <v>106</v>
       </c>
       <c r="F78" s="2"/>
       <c r="G78" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A79" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="B79" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="C79" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D79" s="2">
+        <v>4</v>
+      </c>
+      <c r="E79" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="F79" s="2"/>
+      <c r="G79" s="2" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A80" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="B80" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C80" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D80" s="2">
+        <v>1</v>
+      </c>
+      <c r="E80" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="F80" s="2"/>
+      <c r="G80" s="2" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="79" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="B79" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="C79" s="2" t="s">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A81" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="D79" s="2">
-        <v>2</v>
-      </c>
-      <c r="E79" s="2"/>
-      <c r="F79" s="2" t="s">
+      <c r="B81" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C81" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="D81" s="2">
+        <v>2</v>
+      </c>
+      <c r="E81" s="2"/>
+      <c r="F81" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="G79" s="2" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="80" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="2"/>
-      <c r="B80" s="2"/>
-      <c r="C80" s="2"/>
-      <c r="D80" s="2"/>
-      <c r="E80" s="2"/>
-      <c r="F80" s="2"/>
-      <c r="G80" s="2"/>
-    </row>
-    <row r="81" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="2"/>
-      <c r="B81" s="2"/>
-      <c r="C81" s="2"/>
-      <c r="D81" s="2"/>
-      <c r="E81" s="2"/>
-      <c r="F81" s="2"/>
-      <c r="G81" s="2"/>
-    </row>
-    <row r="82" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="7" t="s">
-        <v>139</v>
-      </c>
-      <c r="B82" s="7"/>
-      <c r="C82" s="7"/>
-      <c r="D82" s="7"/>
-      <c r="E82" s="7"/>
-      <c r="F82" s="7"/>
-      <c r="G82" s="7"/>
+      <c r="G81" s="2" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A82" s="3"/>
+      <c r="B82" s="3"/>
+      <c r="C82" s="3"/>
+      <c r="D82" s="3"/>
+      <c r="E82" s="3"/>
+      <c r="F82" s="3"/>
+      <c r="G82" s="3"/>
     </row>
     <row r="83" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="4" t="s">
+      <c r="A83" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="B83" s="6"/>
+      <c r="C83" s="6"/>
+      <c r="D83" s="6"/>
+      <c r="E83" s="6"/>
+      <c r="F83" s="6"/>
+      <c r="G83" s="6"/>
+    </row>
+    <row r="84" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A84" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B83" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C83" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D83" s="4" t="s">
+      <c r="B84" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C84" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D84" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E83" s="4" t="s">
+      <c r="E84" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F83" s="4" t="s">
+      <c r="F84" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="G83" s="4" t="s">
+      <c r="G84" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="84" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="2" t="s">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A85" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B84" s="2" t="s">
+      <c r="B85" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C84" s="2" t="s">
+      <c r="C85" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D84" s="2">
-        <v>1</v>
-      </c>
-      <c r="E84" s="2" t="s">
+      <c r="D85" s="2">
+        <v>1</v>
+      </c>
+      <c r="E85" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="F84" s="2"/>
-      <c r="G84" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="85" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B85" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C85" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D85" s="2">
-        <v>2</v>
-      </c>
-      <c r="E85" s="2" t="s">
-        <v>38</v>
       </c>
       <c r="F85" s="2"/>
       <c r="G85" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A86" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B86" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C86" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D86" s="2">
+        <v>2</v>
+      </c>
+      <c r="E86" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F86" s="2"/>
+      <c r="G86" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="86" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="2"/>
-      <c r="B86" s="2"/>
-      <c r="C86" s="2" t="s">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A87" s="2"/>
+      <c r="B87" s="2"/>
+      <c r="C87" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="D86" s="2">
-        <v>1</v>
-      </c>
-      <c r="E86" s="2"/>
-      <c r="F86" s="2" t="s">
+      <c r="D87" s="2">
+        <v>1</v>
+      </c>
+      <c r="E87" s="2"/>
+      <c r="F87" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="G86" s="2" t="s">
+      <c r="G87" s="2" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="87" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="3"/>
-      <c r="B87" s="3"/>
-      <c r="C87" s="3"/>
-      <c r="D87" s="3"/>
-      <c r="E87" s="3"/>
-      <c r="F87" s="3"/>
-      <c r="G87" s="3"/>
-    </row>
-    <row r="88" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="7" t="s">
-        <v>140</v>
-      </c>
-      <c r="B88" s="7"/>
-      <c r="C88" s="7"/>
-      <c r="D88" s="7"/>
-      <c r="E88" s="7"/>
-      <c r="F88" s="7"/>
-      <c r="G88" s="7"/>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A88" s="3"/>
+      <c r="B88" s="3"/>
+      <c r="C88" s="3"/>
+      <c r="D88" s="3"/>
+      <c r="E88" s="3"/>
+      <c r="F88" s="3"/>
+      <c r="G88" s="3"/>
     </row>
     <row r="89" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="4" t="s">
+      <c r="A89" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="B89" s="6"/>
+      <c r="C89" s="6"/>
+      <c r="D89" s="6"/>
+      <c r="E89" s="6"/>
+      <c r="F89" s="6"/>
+      <c r="G89" s="6"/>
+    </row>
+    <row r="90" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A90" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B89" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C89" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D89" s="4" t="s">
+      <c r="B90" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C90" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D90" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E89" s="4" t="s">
+      <c r="E90" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F89" s="4" t="s">
+      <c r="F90" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="G89" s="4" t="s">
+      <c r="G90" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="90" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="2" t="s">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A91" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B90" s="2" t="s">
+      <c r="B91" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C90" s="2" t="s">
+      <c r="C91" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D90" s="2">
-        <v>1</v>
-      </c>
-      <c r="E90" s="2" t="s">
+      <c r="D91" s="2">
+        <v>1</v>
+      </c>
+      <c r="E91" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="F90" s="2"/>
-      <c r="G90" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="91" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B91" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C91" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D91" s="2">
-        <v>2</v>
-      </c>
-      <c r="E91" s="2" t="s">
-        <v>38</v>
       </c>
       <c r="F91" s="2"/>
       <c r="G91" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A92" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B92" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C92" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D92" s="2">
+        <v>2</v>
+      </c>
+      <c r="E92" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F92" s="2"/>
+      <c r="G92" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="92" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="11" t="s">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A93" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="B92" s="2" t="s">
+      <c r="B93" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="C92" s="2" t="s">
+      <c r="C93" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="D92" s="2">
-        <v>1</v>
-      </c>
-      <c r="E92" s="2" t="s">
+      <c r="D93" s="2">
+        <v>1</v>
+      </c>
+      <c r="E93" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="F92" s="2"/>
-      <c r="G92" t="s">
+      <c r="F93" s="2"/>
+      <c r="G93" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="93" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="2"/>
-      <c r="B93" s="2"/>
-      <c r="C93" s="2" t="s">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A94" s="2"/>
+      <c r="B94" s="2"/>
+      <c r="C94" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="D93" s="2">
-        <v>2</v>
-      </c>
-      <c r="E93" s="2"/>
-      <c r="F93" s="2"/>
-      <c r="G93" s="2" t="s">
+      <c r="D94" s="2">
+        <v>2</v>
+      </c>
+      <c r="E94" s="2"/>
+      <c r="F94" s="2"/>
+      <c r="G94" s="2" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="94" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="3"/>
-      <c r="B94" s="3"/>
-      <c r="C94" s="3"/>
-      <c r="D94" s="3"/>
-      <c r="E94" s="3"/>
-      <c r="F94" s="3"/>
-      <c r="G94" s="3"/>
-    </row>
-    <row r="95" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="7" t="s">
-        <v>145</v>
-      </c>
-      <c r="B95" s="7"/>
-      <c r="C95" s="7"/>
-      <c r="D95" s="7"/>
-      <c r="E95" s="7"/>
-      <c r="F95" s="7"/>
-      <c r="G95" s="7"/>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A95" s="3"/>
+      <c r="B95" s="3"/>
+      <c r="C95" s="3"/>
+      <c r="D95" s="3"/>
+      <c r="E95" s="3"/>
+      <c r="F95" s="3"/>
+      <c r="G95" s="3"/>
     </row>
     <row r="96" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="4" t="s">
+      <c r="A96" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="B96" s="6"/>
+      <c r="C96" s="6"/>
+      <c r="D96" s="6"/>
+      <c r="E96" s="6"/>
+      <c r="F96" s="6"/>
+      <c r="G96" s="6"/>
+    </row>
+    <row r="97" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A97" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B96" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C96" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D96" s="4" t="s">
+      <c r="B97" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C97" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D97" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E96" s="4" t="s">
+      <c r="E97" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F96" s="4" t="s">
+      <c r="F97" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="G96" s="4" t="s">
+      <c r="G97" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="97" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="2" t="s">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A98" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B97" s="2" t="s">
+      <c r="B98" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C97" s="2" t="s">
+      <c r="C98" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D97" s="2">
-        <v>1</v>
-      </c>
-      <c r="E97" s="2" t="s">
+      <c r="D98" s="2">
+        <v>1</v>
+      </c>
+      <c r="E98" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="F97" s="2"/>
-      <c r="G97" s="2" t="s">
+      <c r="F98" s="2"/>
+      <c r="G98" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="98" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A98" s="2"/>
-      <c r="B98" s="2"/>
-      <c r="C98" s="2" t="s">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A99" s="2"/>
+      <c r="B99" s="2"/>
+      <c r="C99" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="D98" s="2">
+      <c r="D99" s="2">
         <v>4</v>
       </c>
-      <c r="E98" s="2"/>
-      <c r="F98" s="2" t="s">
+      <c r="E99" s="2"/>
+      <c r="F99" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="G98" s="10" t="s">
+      <c r="G99" s="2" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="99" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="3"/>
-      <c r="B99" s="3"/>
-      <c r="C99" s="3"/>
-      <c r="D99" s="3"/>
-      <c r="E99" s="3"/>
-      <c r="F99" s="3"/>
-      <c r="G99" s="3"/>
-    </row>
-    <row r="100" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="7" t="s">
-        <v>156</v>
-      </c>
-      <c r="B100" s="7"/>
-      <c r="C100" s="7"/>
-      <c r="D100" s="7"/>
-      <c r="E100" s="7"/>
-      <c r="F100" s="7"/>
-      <c r="G100" s="7"/>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A100" s="3"/>
+      <c r="B100" s="3"/>
+      <c r="C100" s="3"/>
+      <c r="D100" s="3"/>
+      <c r="E100" s="3"/>
+      <c r="F100" s="3"/>
+      <c r="G100" s="3"/>
     </row>
     <row r="101" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A101" s="4" t="s">
+      <c r="A101" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="B101" s="6"/>
+      <c r="C101" s="6"/>
+      <c r="D101" s="6"/>
+      <c r="E101" s="6"/>
+      <c r="F101" s="6"/>
+      <c r="G101" s="6"/>
+    </row>
+    <row r="102" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A102" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B101" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C101" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D101" s="4" t="s">
+      <c r="B102" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C102" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D102" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E101" s="4" t="s">
+      <c r="E102" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F101" s="4" t="s">
+      <c r="F102" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="G101" s="4" t="s">
+      <c r="G102" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="102" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A102" s="2" t="s">
+    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A103" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B102" s="2" t="s">
+      <c r="B103" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C102" s="2" t="s">
+      <c r="C103" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D102" s="2">
-        <v>1</v>
-      </c>
-      <c r="E102" s="2" t="s">
+      <c r="D103" s="2">
+        <v>1</v>
+      </c>
+      <c r="E103" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="F102" s="2"/>
-      <c r="G102" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="103" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A103" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B103" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C103" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D103" s="2">
-        <v>4</v>
-      </c>
-      <c r="E103" s="2" t="s">
-        <v>83</v>
       </c>
       <c r="F103" s="2"/>
       <c r="G103" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A104" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B104" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C104" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D104" s="2">
+        <v>4</v>
+      </c>
+      <c r="E104" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="F104" s="2"/>
+      <c r="G104" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="104" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="2"/>
-      <c r="B104" s="2"/>
-      <c r="C104" s="2" t="s">
+    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A105" s="2"/>
+      <c r="B105" s="2"/>
+      <c r="C105" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="D104" s="2">
-        <v>2</v>
-      </c>
-      <c r="E104" s="2"/>
-      <c r="F104" s="2" t="s">
+      <c r="D105" s="2">
+        <v>2</v>
+      </c>
+      <c r="E105" s="2"/>
+      <c r="F105" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="G104" s="2" t="s">
+      <c r="G105" s="2" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="105" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A105" s="3"/>
-      <c r="B105" s="3"/>
-      <c r="C105" s="3"/>
-      <c r="D105" s="3"/>
-      <c r="E105" s="3"/>
-      <c r="F105" s="3"/>
-      <c r="G105" s="3"/>
-    </row>
-    <row r="106" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A106" s="7" t="s">
-        <v>157</v>
-      </c>
-      <c r="B106" s="7"/>
-      <c r="C106" s="7"/>
-      <c r="D106" s="7"/>
-      <c r="E106" s="7"/>
-      <c r="F106" s="7"/>
-      <c r="G106" s="7"/>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A106" s="3"/>
+      <c r="B106" s="3"/>
+      <c r="C106" s="3"/>
+      <c r="D106" s="3"/>
+      <c r="E106" s="3"/>
+      <c r="F106" s="3"/>
+      <c r="G106" s="3"/>
     </row>
     <row r="107" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A107" s="4" t="s">
+      <c r="A107" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="B107" s="6"/>
+      <c r="C107" s="6"/>
+      <c r="D107" s="6"/>
+      <c r="E107" s="6"/>
+      <c r="F107" s="6"/>
+      <c r="G107" s="6"/>
+    </row>
+    <row r="108" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A108" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B107" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C107" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D107" s="4" t="s">
+      <c r="B108" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C108" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D108" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E107" s="4" t="s">
+      <c r="E108" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F107" s="4" t="s">
+      <c r="F108" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="G107" s="4" t="s">
+      <c r="G108" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="108" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A108" s="2" t="s">
+    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A109" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B108" s="2" t="s">
+      <c r="B109" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C108" s="2" t="s">
+      <c r="C109" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D108" s="2">
-        <v>1</v>
-      </c>
-      <c r="E108" s="2" t="s">
+      <c r="D109" s="2">
+        <v>1</v>
+      </c>
+      <c r="E109" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="F108" s="2"/>
-      <c r="G108" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="109" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A109" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B109" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C109" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D109" s="2">
-        <v>4</v>
-      </c>
-      <c r="E109" s="2" t="s">
-        <v>92</v>
       </c>
       <c r="F109" s="2"/>
       <c r="G109" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="110" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A110" s="2" t="s">
-        <v>84</v>
+        <v>9</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>86</v>
+        <v>8</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>88</v>
+        <v>7</v>
       </c>
       <c r="D110" s="2">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E110" s="2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="F110" s="2"/>
       <c r="G110" s="2" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="111" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A111" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D111" s="2">
         <v>1</v>
       </c>
       <c r="E111" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F111" s="2"/>
       <c r="G111" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A112" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B112" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C112" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="D112" s="2">
+        <v>1</v>
+      </c>
+      <c r="E112" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="F112" s="2"/>
+      <c r="G112" s="2" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="112" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A112" s="2"/>
-      <c r="B112" s="2"/>
-      <c r="C112" s="2" t="s">
+    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A113" s="2"/>
+      <c r="B113" s="2"/>
+      <c r="C113" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="D112" s="2">
-        <v>2</v>
-      </c>
-      <c r="E112" s="2"/>
-      <c r="F112" s="2" t="s">
+      <c r="D113" s="2">
+        <v>2</v>
+      </c>
+      <c r="E113" s="2"/>
+      <c r="F113" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="G112" s="2" t="s">
+      <c r="G113" s="2" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="113" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A113" s="3"/>
-      <c r="B113" s="3"/>
-      <c r="C113" s="3"/>
-      <c r="D113" s="3"/>
-      <c r="E113" s="3"/>
-      <c r="F113" s="3"/>
-      <c r="G113" s="3"/>
-    </row>
-    <row r="114" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A114" s="7" t="s">
-        <v>158</v>
-      </c>
-      <c r="B114" s="7"/>
-      <c r="C114" s="7"/>
-      <c r="D114" s="7"/>
-      <c r="E114" s="7"/>
-      <c r="F114" s="7"/>
-      <c r="G114" s="7"/>
+    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A114" s="3"/>
+      <c r="B114" s="3"/>
+      <c r="C114" s="3"/>
+      <c r="D114" s="3"/>
+      <c r="E114" s="3"/>
+      <c r="F114" s="3"/>
+      <c r="G114" s="3"/>
     </row>
     <row r="115" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A115" s="4" t="s">
+      <c r="A115" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="B115" s="6"/>
+      <c r="C115" s="6"/>
+      <c r="D115" s="6"/>
+      <c r="E115" s="6"/>
+      <c r="F115" s="6"/>
+      <c r="G115" s="6"/>
+    </row>
+    <row r="116" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A116" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B115" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C115" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D115" s="4" t="s">
+      <c r="B116" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C116" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D116" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E115" s="4" t="s">
+      <c r="E116" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F115" s="4" t="s">
+      <c r="F116" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="G115" s="4" t="s">
+      <c r="G116" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="116" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A116" s="2" t="s">
+    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A117" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B116" s="2" t="s">
+      <c r="B117" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C116" s="2" t="s">
+      <c r="C117" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D116" s="2">
-        <v>1</v>
-      </c>
-      <c r="E116" s="2" t="s">
+      <c r="D117" s="2">
+        <v>1</v>
+      </c>
+      <c r="E117" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="F116" s="2"/>
-      <c r="G116" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="117" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A117" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B117" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C117" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D117" s="2">
-        <v>4</v>
-      </c>
-      <c r="E117" s="2" t="s">
-        <v>46</v>
       </c>
       <c r="F117" s="2"/>
       <c r="G117" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="118" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A118" s="2"/>
-      <c r="B118" s="2"/>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A118" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B118" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="C118" s="2" t="s">
-        <v>80</v>
+        <v>7</v>
       </c>
       <c r="D118" s="2">
-        <v>2</v>
-      </c>
-      <c r="E118" s="2"/>
+        <v>4</v>
+      </c>
+      <c r="E118" s="2" t="s">
+        <v>46</v>
+      </c>
       <c r="F118" s="2"/>
       <c r="G118" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A119" s="2"/>
+      <c r="B119" s="2"/>
+      <c r="C119" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D119" s="2">
+        <v>2</v>
+      </c>
+      <c r="E119" s="2"/>
+      <c r="F119" s="2"/>
+      <c r="G119" s="2" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="119" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A119" s="3"/>
-      <c r="B119" s="3"/>
-      <c r="C119" s="3"/>
-      <c r="D119" s="3"/>
-      <c r="E119" s="3"/>
-      <c r="F119" s="3"/>
-      <c r="G119" s="3"/>
-    </row>
-    <row r="120" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A120" s="7" t="s">
-        <v>159</v>
-      </c>
-      <c r="B120" s="7"/>
-      <c r="C120" s="7"/>
-      <c r="D120" s="7"/>
-      <c r="E120" s="7"/>
-      <c r="F120" s="7"/>
-      <c r="G120" s="7"/>
+    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A120" s="3"/>
+      <c r="B120" s="3"/>
+      <c r="C120" s="3"/>
+      <c r="D120" s="3"/>
+      <c r="E120" s="3"/>
+      <c r="F120" s="3"/>
+      <c r="G120" s="3"/>
     </row>
     <row r="121" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A121" s="4" t="s">
+      <c r="A121" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="B121" s="6"/>
+      <c r="C121" s="6"/>
+      <c r="D121" s="6"/>
+      <c r="E121" s="6"/>
+      <c r="F121" s="6"/>
+      <c r="G121" s="6"/>
+    </row>
+    <row r="122" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A122" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B121" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C121" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D121" s="4" t="s">
+      <c r="B122" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C122" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D122" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E121" s="4" t="s">
+      <c r="E122" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F121" s="4" t="s">
+      <c r="F122" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="G121" s="4" t="s">
+      <c r="G122" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="122" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A122" s="2" t="s">
+    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A123" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B122" s="2" t="s">
+      <c r="B123" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C122" s="2" t="s">
+      <c r="C123" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D122" s="2">
-        <v>1</v>
-      </c>
-      <c r="E122" s="2" t="s">
+      <c r="D123" s="2">
+        <v>1</v>
+      </c>
+      <c r="E123" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="F122" s="2"/>
-      <c r="G122" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="123" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A123" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B123" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C123" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D123" s="2">
-        <v>3</v>
-      </c>
-      <c r="E123" s="2" t="s">
-        <v>38</v>
       </c>
       <c r="F123" s="2"/>
       <c r="G123" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A124" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B124" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C124" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D124" s="2">
+        <v>3</v>
+      </c>
+      <c r="E124" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F124" s="2"/>
+      <c r="G124" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="124" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A124" s="2"/>
-      <c r="B124" s="2"/>
-      <c r="C124" s="2" t="s">
+    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A125" s="2"/>
+      <c r="B125" s="2"/>
+      <c r="C125" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="D124" s="2">
-        <v>2</v>
-      </c>
-      <c r="E124" s="2"/>
-      <c r="F124" s="2" t="s">
+      <c r="D125" s="2">
+        <v>2</v>
+      </c>
+      <c r="E125" s="2"/>
+      <c r="F125" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="G124" s="2" t="s">
+      <c r="G125" s="2" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="125" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A125" s="3"/>
-      <c r="B125" s="3"/>
-      <c r="C125" s="3"/>
-      <c r="D125" s="3"/>
-      <c r="E125" s="3"/>
-      <c r="F125" s="3"/>
-      <c r="G125" s="3"/>
-    </row>
-    <row r="126" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A126" s="7" t="s">
-        <v>163</v>
-      </c>
-      <c r="B126" s="7"/>
-      <c r="C126" s="7"/>
-      <c r="D126" s="7"/>
-      <c r="E126" s="7"/>
-      <c r="F126" s="7"/>
-      <c r="G126" s="7"/>
+    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A126" s="3"/>
+      <c r="B126" s="3"/>
+      <c r="C126" s="3"/>
+      <c r="D126" s="3"/>
+      <c r="E126" s="3"/>
+      <c r="F126" s="3"/>
+      <c r="G126" s="3"/>
     </row>
     <row r="127" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A127" s="4" t="s">
+      <c r="A127" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="B127" s="6"/>
+      <c r="C127" s="6"/>
+      <c r="D127" s="6"/>
+      <c r="E127" s="6"/>
+      <c r="F127" s="6"/>
+      <c r="G127" s="6"/>
+    </row>
+    <row r="128" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A128" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B127" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C127" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D127" s="4" t="s">
+      <c r="B128" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C128" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D128" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E127" s="4" t="s">
+      <c r="E128" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F127" s="4" t="s">
+      <c r="F128" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="G127" s="4" t="s">
+      <c r="G128" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="128" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A128" s="2" t="s">
+    <row r="129" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A129" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B128" s="2" t="s">
+      <c r="B129" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C128" s="2" t="s">
+      <c r="C129" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D128" s="2">
-        <v>1</v>
-      </c>
-      <c r="E128" s="2" t="s">
+      <c r="D129" s="2">
+        <v>1</v>
+      </c>
+      <c r="E129" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="F128" s="2"/>
-      <c r="G128" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="129" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A129" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B129" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C129" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D129" s="2">
-        <v>3</v>
-      </c>
-      <c r="E129" s="2" t="s">
-        <v>94</v>
       </c>
       <c r="F129" s="2"/>
       <c r="G129" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="130" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A130" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B130" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C130" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D130" s="2">
+        <v>3</v>
+      </c>
+      <c r="E130" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="F130" s="2"/>
+      <c r="G130" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="130" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A130" s="2"/>
-      <c r="B130" s="2"/>
-      <c r="C130" s="2" t="s">
+    <row r="131" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A131" s="2"/>
+      <c r="B131" s="2"/>
+      <c r="C131" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="D130" s="2">
-        <v>1</v>
-      </c>
-      <c r="E130" s="2"/>
-      <c r="F130" s="2"/>
-      <c r="G130" s="10" t="s">
+      <c r="D131" s="2">
+        <v>1</v>
+      </c>
+      <c r="E131" s="2"/>
+      <c r="F131" s="2"/>
+      <c r="G131" s="2" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="131" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A131" s="3"/>
-      <c r="B131" s="3"/>
-      <c r="C131" s="3"/>
-      <c r="D131" s="3"/>
-      <c r="E131" s="3"/>
-      <c r="F131" s="3"/>
-      <c r="G131" s="3"/>
-    </row>
-    <row r="132" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A132" s="7" t="s">
-        <v>160</v>
-      </c>
-      <c r="B132" s="7"/>
-      <c r="C132" s="7"/>
-      <c r="D132" s="7"/>
-      <c r="E132" s="7"/>
-      <c r="F132" s="7"/>
-      <c r="G132" s="7"/>
+    <row r="132" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A132" s="3"/>
+      <c r="B132" s="3"/>
+      <c r="C132" s="3"/>
+      <c r="D132" s="3"/>
+      <c r="E132" s="3"/>
+      <c r="F132" s="3"/>
+      <c r="G132" s="3"/>
     </row>
     <row r="133" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A133" s="4" t="s">
+      <c r="A133" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="B133" s="6"/>
+      <c r="C133" s="6"/>
+      <c r="D133" s="6"/>
+      <c r="E133" s="6"/>
+      <c r="F133" s="6"/>
+      <c r="G133" s="6"/>
+    </row>
+    <row r="134" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A134" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B133" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C133" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D133" s="4" t="s">
+      <c r="B134" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C134" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D134" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E133" s="4" t="s">
+      <c r="E134" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F133" s="4" t="s">
+      <c r="F134" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="G133" s="4" t="s">
+      <c r="G134" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="134" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A134" s="2" t="s">
+    <row r="135" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A135" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B134" s="2" t="s">
+      <c r="B135" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C134" s="2" t="s">
+      <c r="C135" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D134" s="2">
-        <v>1</v>
-      </c>
-      <c r="E134" s="2" t="s">
+      <c r="D135" s="2">
+        <v>1</v>
+      </c>
+      <c r="E135" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="F134" s="2"/>
-      <c r="G134" s="2" t="s">
+      <c r="F135" s="2"/>
+      <c r="G135" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="135" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A135" s="2"/>
-      <c r="B135" s="2"/>
-      <c r="C135" s="2" t="s">
+    <row r="136" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A136" s="2"/>
+      <c r="B136" s="2"/>
+      <c r="C136" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="D135" s="2">
-        <v>2</v>
-      </c>
-      <c r="E135" s="2"/>
-      <c r="F135" s="2" t="s">
+      <c r="D136" s="2">
+        <v>2</v>
+      </c>
+      <c r="E136" s="2"/>
+      <c r="F136" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="G135" s="2" t="s">
+      <c r="G136" s="2" t="s">
         <v>68</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="G62:G63"/>
+  </mergeCells>
   <hyperlinks>
-    <hyperlink ref="G7" r:id="rId1"/>
-    <hyperlink ref="G3" r:id="rId2"/>
-    <hyperlink ref="G53" r:id="rId3"/>
-    <hyperlink ref="G29" r:id="rId4"/>
-    <hyperlink ref="G84" r:id="rId5"/>
-    <hyperlink ref="G116" r:id="rId6"/>
-    <hyperlink ref="G66" r:id="rId7"/>
-    <hyperlink ref="G67" r:id="rId8"/>
-    <hyperlink ref="G117" r:id="rId9"/>
-    <hyperlink ref="G85" r:id="rId10"/>
-    <hyperlink ref="G30" r:id="rId11"/>
-    <hyperlink ref="G54" r:id="rId12"/>
-    <hyperlink ref="G31" r:id="rId13"/>
-    <hyperlink ref="G55" r:id="rId14"/>
-    <hyperlink ref="G5" r:id="rId15"/>
-    <hyperlink ref="G6" r:id="rId16"/>
-    <hyperlink ref="G68" r:id="rId17"/>
-    <hyperlink ref="G70" r:id="rId18"/>
-    <hyperlink ref="G56" r:id="rId19"/>
-    <hyperlink ref="G118" r:id="rId20"/>
-    <hyperlink ref="G86" r:id="rId21"/>
-    <hyperlink ref="G32" r:id="rId22"/>
-    <hyperlink ref="G33" r:id="rId23"/>
-    <hyperlink ref="G11" r:id="rId24"/>
-    <hyperlink ref="G12" r:id="rId25"/>
-    <hyperlink ref="G13" r:id="rId26"/>
-    <hyperlink ref="G17" r:id="rId27"/>
-    <hyperlink ref="G18" r:id="rId28"/>
-    <hyperlink ref="G19" r:id="rId29"/>
-    <hyperlink ref="G90" r:id="rId30"/>
-    <hyperlink ref="G91" r:id="rId31"/>
-    <hyperlink ref="G97" r:id="rId32"/>
-    <hyperlink ref="G48" r:id="rId33"/>
-    <hyperlink ref="G49" r:id="rId34"/>
-    <hyperlink ref="G135" r:id="rId35"/>
-    <hyperlink ref="G134" r:id="rId36"/>
-    <hyperlink ref="G108" r:id="rId37"/>
-    <hyperlink ref="G109" r:id="rId38"/>
-    <hyperlink ref="G102" r:id="rId39"/>
-    <hyperlink ref="G103" r:id="rId40"/>
-    <hyperlink ref="G23" r:id="rId41"/>
-    <hyperlink ref="G24" r:id="rId42"/>
-    <hyperlink ref="G128" r:id="rId43"/>
-    <hyperlink ref="G129" r:id="rId44"/>
-    <hyperlink ref="G43" r:id="rId45"/>
-    <hyperlink ref="G44" r:id="rId46"/>
-    <hyperlink ref="G37" r:id="rId47"/>
-    <hyperlink ref="G38" r:id="rId48"/>
-    <hyperlink ref="G122" r:id="rId49"/>
-    <hyperlink ref="G123" r:id="rId50"/>
-    <hyperlink ref="G60" r:id="rId51"/>
-    <hyperlink ref="G61" r:id="rId52"/>
-    <hyperlink ref="G104" r:id="rId53"/>
-    <hyperlink ref="G112" r:id="rId54"/>
-    <hyperlink ref="G124" r:id="rId55"/>
-    <hyperlink ref="G93" r:id="rId56"/>
-    <hyperlink ref="G76" r:id="rId57"/>
+    <hyperlink ref="G7" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="G3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="G53" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="G29" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="G85" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="G117" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="G67" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="G68" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="G118" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="G86" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="G30" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="G54" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="G31" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="G55" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="G5" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="G6" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="G69" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="G71" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="G56" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="G119" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="G87" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="G32" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="G33" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="G11" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="G12" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="G13" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="G17" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="G18" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="G19" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="G91" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="G92" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="G98" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="G48" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
+    <hyperlink ref="G49" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
+    <hyperlink ref="G136" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
+    <hyperlink ref="G135" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
+    <hyperlink ref="G109" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
+    <hyperlink ref="G110" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
+    <hyperlink ref="G103" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
+    <hyperlink ref="G104" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
+    <hyperlink ref="G23" r:id="rId41" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
+    <hyperlink ref="G24" r:id="rId42" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
+    <hyperlink ref="G129" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
+    <hyperlink ref="G130" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
+    <hyperlink ref="G43" r:id="rId45" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
+    <hyperlink ref="G44" r:id="rId46" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
+    <hyperlink ref="G37" r:id="rId47" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
+    <hyperlink ref="G38" r:id="rId48" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
+    <hyperlink ref="G123" r:id="rId49" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
+    <hyperlink ref="G124" r:id="rId50" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
+    <hyperlink ref="G60" r:id="rId51" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
+    <hyperlink ref="G61" r:id="rId52" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
+    <hyperlink ref="G105" r:id="rId53" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
+    <hyperlink ref="G113" r:id="rId54" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
+    <hyperlink ref="G125" r:id="rId55" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
+    <hyperlink ref="G94" r:id="rId56" xr:uid="{00000000-0004-0000-0000-000037000000}"/>
+    <hyperlink ref="G78" r:id="rId57" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
+    <hyperlink ref="G81" r:id="rId58" xr:uid="{594F7E4B-550B-424A-A9CE-F66035C208C3}"/>
   </hyperlinks>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="39" fitToHeight="0" orientation="landscape" r:id="rId58"/>
+  <pageSetup scale="39" fitToHeight="0" orientation="landscape" r:id="rId59"/>
+  <rowBreaks count="1" manualBreakCount="1">
+    <brk id="82" max="6" man="1"/>
+  </rowBreaks>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:A66"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="148" style="13" customWidth="1"/>
+    <col min="1" max="1" width="148" style="11" customWidth="1"/>
     <col min="2" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="10" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:1" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="3" spans="1:1" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="11" t="s">
+    <row r="4" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="10" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="4" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="12" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="11" t="s">
+    <row r="7" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="10" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" s="9" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" s="9" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="10" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" s="9" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" s="9" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="10" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" s="9" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" s="9" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="10" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="9" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="9" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="9" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="9" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="10" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" s="9" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" s="9" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="10" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" s="9" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" s="9" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="10" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" s="9" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" s="9" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="10" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" s="9" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" s="9" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" s="9" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" s="9" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" s="9" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="10" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" s="9" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A39" s="9" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="10" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="6" spans="1:1" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="11" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="12" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="11" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="11" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="12" t="s">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" s="9" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" s="9" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="10" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" s="9" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45" s="9" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="10" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47" s="9" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48" s="9" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="10" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="11" spans="1:1" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="11" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="11" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="12" t="s">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" s="9" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" s="9" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="10" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53" s="9" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54" s="9" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" s="5" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="10" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A56" s="9" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A57" s="9" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="10" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A59" s="9" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A60" s="9" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="10" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="14" spans="1:1" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="11" t="s">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A62" s="9" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A63" s="9" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="15" spans="1:1" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="11" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="12" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="11" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="11" t="s">
+    <row r="64" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="10" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65" s="9" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66" s="9" t="s">
         <v>169</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="12" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="11" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="11" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="12" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="11" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="11" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="12" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="11" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="11" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="12" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="11" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="11" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="12" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="11" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="11" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="11" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="11" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="11" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="12" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="11" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A39" s="11" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="12" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="11" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="11" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="12" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="44" spans="1:1" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="11" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="45" spans="1:1" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="11" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="46" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="12" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="47" spans="1:1" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="11" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="48" spans="1:1" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="11" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="12" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="11" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="51" spans="1:1" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="11" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="52" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="12" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="53" spans="1:1" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="11" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="54" spans="1:1" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="11" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="55" spans="1:1" s="5" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="12" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="56" spans="1:1" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="11" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="57" spans="1:1" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="11" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="58" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="12" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="59" spans="1:1" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="11" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="60" spans="1:1" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="11" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="61" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="12" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="62" spans="1:1" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="11" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="63" spans="1:1" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="11" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="64" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="12" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="65" spans="1:1" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="11" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="66" spans="1:1" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="11" t="s">
-        <v>170</v>
       </c>
     </row>
   </sheetData>

</xml_diff>